<commit_message>
Add write menu method
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\NetBeansProjects\restaurant-management-application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56AD59F-0AFB-48D5-B4B3-55842905FECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD0CB77-2BB3-490F-8E4F-C223D728C283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1F33AB81-9ED0-477A-B264-3B3B472DEDDA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ไก่</t>
   </si>
@@ -42,10 +42,19 @@
     <t>ไข่</t>
   </si>
   <si>
-    <t>พะแนว</t>
-  </si>
-  <si>
-    <t>มาม่า</t>
+    <t>ส้ม</t>
+  </si>
+  <si>
+    <t>โรตี</t>
+  </si>
+  <si>
+    <t>พะแนง</t>
+  </si>
+  <si>
+    <t>หมูปิ้ง</t>
+  </si>
+  <si>
+    <t>แหนม</t>
   </si>
 </sst>
 </file>
@@ -398,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C434D0-C961-44A7-8DE3-41DD6CBEB97F}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,12 +431,44 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
-        <v>5.0</v>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>15.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>